<commit_message>
Updated demonstrator worksheet practices
</commit_message>
<xml_diff>
--- a/static/downloads/AberworksTimesheet.xlsx
+++ b/static/downloads/AberworksTimesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\fbaps-faculty\HR\Timesheets\Template timesheets\2023 - 24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jim\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1DCDC3E-976E-4887-A87F-8CDFB85D70B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0030D3E-A425-487D-84D6-AE21027EDC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="20376" windowHeight="12096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AberWorks Timesheet" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -368,11 +368,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -433,35 +444,38 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,26 +517,39 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,6 +746,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8627FC3B-7265-2D4F-D493-3C3BFFE4DECE}"/>
@@ -770,8 +798,54 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>When completing your timesheet:</a:t>
+            <a:t>Please see https://users.aber.ac.uk/jcf12/teaching/demonstrating/timesheet/ for guidance</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> on completing this timesheet.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1400" b="1" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>Each timesheets should be used for a single module only - fill in a separate timesheet for each module you are demonstrating.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1400" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1400">
@@ -783,349 +857,6 @@
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>* Insert the start and finish time in 24 hour clock format, including the minutes e.g. start time 14:00 finish time * 17:30</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Only claim for work that has actually been completed (you may work up to 15 hours per week) across all AberWorks roles.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>* Students working on a Student Visa will only be able to work hours that remain compliant with their Visa.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>* Submit your hours every month (by the required deadlines as noted below) even if you have only worked a few hours that month. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>* All timesheet claims must be confirmed and signed by the supervisor of the module you are demonstrating for </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>before</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> being submitted for processing </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>via email only</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> to </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
-            <a:t>gsm@aber.ac.uk</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> by the deadline above.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>* Any timesheets received after the deadline will not be processed until the following month</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Payment will be processed so that you will be paid on the last working day of the month following the month you are submitting for.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>*  Avoid accumulating hours as this will have implications on the amount of tax and National Insurance that you pay.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:endParaRPr lang="en-GB" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Head of Department</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> authorisation will be obtained by Glenwen.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:endParaRPr lang="en-GB" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Because the worksheets are submitted electronically, electronic signatures are acceptable. Any printed  worksheets to obtain physical signatures will need</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> to be scanned and emailed to Glenwen</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="0"/>
-          <a:endParaRPr lang="en-GB" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>If you have any questions about timesheets, contact Glenwen on </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
-            </a:rPr>
-            <a:t>gsm@aber.ac.uk</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-GB" sz="1400">
@@ -1151,7 +882,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>V.10.23</a:t>
+            <a:t>V.10.24</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="2400" b="1">
             <a:solidFill>
@@ -1491,8 +1222,8 @@
   </sheetPr>
   <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1512,25 +1243,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="15"/>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
@@ -1540,86 +1271,89 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
       <c r="E5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47"/>
       <c r="H5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="27"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="48"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="27"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="27"/>
-      <c r="J8" s="18"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="61"/>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54" t="s">
+      <c r="D9" s="28"/>
+      <c r="E9" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="54"/>
-      <c r="G9" s="58" t="s">
+      <c r="F9" s="28"/>
+      <c r="G9" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="57"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="59"/>
       <c r="M9" s="17"/>
     </row>
     <row r="10" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="53"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1632,16 +1366,16 @@
       <c r="F10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="59"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
       <c r="M10" s="17"/>
     </row>
     <row r="11" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1663,10 +1397,10 @@
         <v>7</v>
       </c>
       <c r="H11" s="7"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="27"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="31"/>
       <c r="M11" s="17"/>
     </row>
     <row r="12" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1688,10 +1422,10 @@
         <v>7</v>
       </c>
       <c r="H12" s="7"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="27"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="31"/>
       <c r="M12" s="17"/>
     </row>
     <row r="13" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,10 +1447,10 @@
         <v>7</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="27"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="31"/>
       <c r="M13" s="17"/>
     </row>
     <row r="14" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1738,10 +1472,10 @@
         <v>7</v>
       </c>
       <c r="H14" s="7"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="27"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="31"/>
       <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1763,10 +1497,10 @@
         <v>7</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="27"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="31"/>
       <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1788,8 +1522,8 @@
         <v>7</v>
       </c>
       <c r="H16" s="7"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="31"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="17"/>
@@ -1813,8 +1547,8 @@
         <v>7</v>
       </c>
       <c r="H17" s="7"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="31"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="17"/>
@@ -1838,8 +1572,8 @@
         <v>7</v>
       </c>
       <c r="H18" s="7"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="31"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="17"/>
@@ -1863,8 +1597,8 @@
         <v>7</v>
       </c>
       <c r="H19" s="7"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="31"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="17"/>
@@ -1888,10 +1622,10 @@
         <v>7</v>
       </c>
       <c r="H20" s="7"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="27"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
       <c r="M20" s="17"/>
     </row>
     <row r="21" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1915,10 +1649,10 @@
         <v>7</v>
       </c>
       <c r="H21" s="7"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="L21" s="27"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="31"/>
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1940,20 +1674,20 @@
         <v>7</v>
       </c>
       <c r="H22" s="7"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="27"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="31"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="56"/>
       <c r="G23" s="11" t="s">
         <v>7</v>
       </c>
@@ -1984,16 +1718,16 @@
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="E26" s="28" t="s">
+      <c r="B26" s="38"/>
+      <c r="C26" s="39"/>
+      <c r="E26" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
       <c r="H26" s="24"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
@@ -2004,13 +1738,13 @@
       <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="31"/>
       <c r="E27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="27"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="31"/>
       <c r="H27" s="25"/>
       <c r="I27" s="23"/>
       <c r="J27" s="23"/>
@@ -2021,13 +1755,13 @@
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="31"/>
       <c r="E28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="26"/>
-      <c r="G28" s="27"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="31"/>
       <c r="H28" s="25"/>
       <c r="I28" s="23"/>
       <c r="J28" s="23"/>
@@ -2049,13 +1783,23 @@
       <c r="F31" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="D2:H3"/>
+  <mergeCells count="37">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="I12:L12"/>
     <mergeCell ref="I13:L13"/>
@@ -2070,22 +1814,13 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="I22:L22"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I8:J9"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="43" orientation="landscape" r:id="rId1"/>

</xml_diff>